<commit_message>
UI Adjustment - top and wide
</commit_message>
<xml_diff>
--- a/pbm_output.xlsx
+++ b/pbm_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,507 +456,402 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Case Owner</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>PBM_Tag</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2008416</v>
+        <v>1990922</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BMC Digital Workplace 22.1.06 - "On behalf of" issue</t>
+          <t>Creating Change request from Smart IT not showing in DWP for customer.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hello, We are facing an issue regarding the "Request on behalf of" functionality in DWP and we want to understand why this is happening and how can it be corrected. Right after submitting the Service Request on behalf of a user from another company than the one making the request it immediately goes into "Failed" status, mentioning the error "Contact should be type of Customer or Employee." We have already checked from Workflow side, all the blocks and variables seems to be in order. We have attached the filter and process logs (in the same file) and DWPC logs for better clarity regarding what is happening. Please look into it and let us know what can be done to solve this.</t>
+          <t>When creating change request from Smart IT or Mid Tier, and selects the customer (requested for) user the corresponding request does not show in DWP portal for the customer. The request is showing in DWP for the submitter. Please see attached document for details. Our DWPC is still in pre-production state but will soon be migrated to production. Helix ITSM version 23.3.04.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Problem: BMC Digital Workplace 22.1.06 - "On behalf of" issue 3WE What: BMC Digital Workplace 22.1.06 - "On behalf of" issue Where: DWP version 22.1.06 When: Issue reported on 07/07 Extent: Functionality ---------------------------------------------------------------------------------------------------- Action Taken: - Solution provided in bookmarked mail - Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
+          <t>Problem: Creating Change request from Smart IT not showing in DWP for customer. 3WE What: When creating change request from Smart IT or Mid Tier, and selects the customer (requested for) user the corresponding request does not show in DWP portal for the customer. The request is showing in DWP for the submitter. Where: Onprem - DWP version 23.3.04 When: Issue reported on 04/06 Extent: Requested for users affected. Steps to Reproduce: - Log in to Smart IT as a support agent or change coordinator. - Create a new Change Request: - Go to Create New &gt; Change Request. - Fill in the required details. - In the Customer field, select an end user. - Submit the change. - Check the associated Request (REQ): - Go to the Activities tab or related records to locate the linked Service Request (REQ). - Open the REQ record. - Observe the "Customer" field in the REQ: - Note that the submitter (you) is set as the requester instead of the end user specified in the Change. - Log in to Digital Workplace (DWP) as the end user: - Check My Activity &gt; Requests. - Verify visibility: - Confirm that the Request is not visible to the end user. - Confirm that the REQ number exists but is only accessible by the submitter. ---------------------------------------------------------------------------------------------------- Action Taken: 04/06; 1. R&amp;D discussion: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1749024890414?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1749024890414&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1749024890414 06/06; 1. Unable to replicate the issue in our test env. 2. Issue is from SRM side and is happening because submitter (you) is set as the requester instead of the end user specified in the Change. 09/06; 1. Need to capture server side logs and check why and how submitter (you) is set as the requester instead of the end user specified in the Change. 2. Asked for teams call time slots for capturing logs 09/06/2025 &gt;&gt; Call is scheduled with the customer 12/06/2025 &gt;&gt; Details were discussed over the call with the customer on the 9th June 2025 and below update is shared with the customer ? During the session, we reproduced the issue by creating a change request on behalf of the user "User 02", with "Martin Lindholm" submitting the request on their behalf. ? While raising the change request, both the Requested For and Requested By fields appeared as "Martin Lindholm". Ideally, the Requested For should reflect "User 02". Additionally, upon reviewing the request, the Customer and Submitted By fields also showed as "Martin Lindholm", whereas we would expect the Customer to be "User 02", as per you have mentioned. ? We also checked the Active Events section in Digital Workplace for "User 02", where the change request and its associated REQ ID should ideally be visible. Initially, we assumed this visibility issue might be due to the use of a custom studio page instead of the out-of-the-box My Activity page, but that turned out not to be the cause. ? Interestingly, the change request raised on behalf of "User 02" is instead visible under the My Activity page of "Martin Lindholm". ? We wrapped up the call by kindly requesting your support in sharing the relevant logs to help us investigate further. ? Thank you once again for promptly sharing the logs. I will be reviewing them thoroughly and will update you with our findings. ? Customer shared the details with us and the logs, we will review it and share the update with the customer 19/06/2025 &gt;&gt; Upon reviewing the DWP logs, I found the following error snippet: Caused by: com.bmc.arsys.server.rx.services.RxFrameworkException: [ERROR (307): Required field cannot be blank.; dwp:DeviceToken : UserPk] 	at com.bmc.arsys.server.rx.services.record.repository.ArRecordInstanceRepository.createRecordInstance(ArRecordInstanceRepository.java:303) 	at com.bmc.arsys.server.rx.services.record.RecordServiceImpl.createRecordInstance(RecordServiceImpl.java:363) 	at com.bmc.dwp.persistence.service.RxPersistService.createOrUpdate(RxPersistService.java:443) 	... 102 common frames omitted &gt;&gt; Based on this, it appears that when the "User details" are being pushed during Change Request creation, the "UserPk" for "User 02" is missing. As a result, the system is skipping "User 02's" details and instead showing "Martin Lindholm" in the Requested For section. &gt;&gt; To address this, I kindly request you to follow the steps below: ? Navigate to: Innovation Studio &gt; Digital Workplace &gt; dwp:UserDetails. Use the filter to search by UserID ? Copy the corresponding ID. (Please refer to the screenshot below.) ? Then go to: Innovation Studio &gt; Digital Workplace &gt; dwp:DeviceToken. Paste the copied ID into the UserPk field in the filter ? Click on Apply ? Validate both the UserPk and Token fields. (Refer to the screenshot below.) ? If you're unable to find the entry using the "UserPk", try searching by the Token value, in your case, it would likely be: "dummyToken:User 02". Then, update the UserPk field with the ID you obtained from the "UserDetails" table and Save. &gt;&gt; Essentially, either the UserPk or the Token value may be missing or mismatched, so this cross-check and correction should help resolve the issue. If the record is not present then we will need to create new one for "User 02". &gt;&gt; I?d like to mention that while reviewing the API/SQL/FLTR logs, I didn?t find any indication of incorrect data being pushed. Therefore, based on the DWP logs, I believe this might be the cause. &gt;&gt; Awaiting for customer to respond 01/07/2025 &gt;&gt; Had a discussion internal and found the Defect: https://jira.bmc.com/browse/DRSMX-115766, below update is shared with the customer -- I?ve discussed this internally with our team, and I?d like to confirm that this is a known issue. In fact, I was able to locate an active defect that directly relates to this specific use-case. This is currently targeted to be addressed in the 25.4.00 version. -- The current behavior is that both Requested For and Requested By appear as the submitter (when submitting on behalf of someone else). However, the expected behavior is that Requested For should reflect the user for whom the request is raised, and Requested By should reflect the one who submitted it. -- This fix will ensure that when a CRQ, Incident, or Work Order creates either a DWPC Request ID or an SRM Request ID, the Requested For and Requested By fields will be correctly populated. &gt;&gt; Awaiting for customer to respond 02/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 04/07/2025 &gt;&gt; Customer agreed to close the case &gt;&gt; We have shared the Defect ID with the customer and closure email is sent &gt;&gt; Closing this case today ---------------------------------------------------------------------------------------------------- Action Plan: Need to schedule call with customer and get logs. ? Need to review the logs and check the issue further &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Request:Check user roles and company associations for 'On behalf of' requests.:Educate</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Request:Change request not visible due to request visibility settings.:R&amp;D</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2008401</v>
+        <v>1991211</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ticket status issue</t>
+          <t>VZINC0001575726: DWP My Activity Internal Server Error when opening approval as delegate</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dear, We have one of our VIP users that is claiming that some of his tickets are still on pending (see attachment) on his Remedy profile while those tickets are closed on Service Desk side. Could you please check why those tickets are not on status solved/closed on his profile?</t>
+          <t>Issue reported by our client ---------------------------------------- When user would like to open a delegate approval from a user who has left the company. The delegate user get internal server error. Steps to reproduct Login with user in DWP: donnersj My Activity Open the approval request REQ000000602441 Please investigate and fix this issue. Probably this is because the original approver (Maurice Leinarts) left the company and the profile is on Delete. Please fix the rootcause and not only these tickets. This needs to be approved/rejected by delegates. Application should handle the use case when an user leaves the company and has still assigned approvals. Tiberone Analysis ------------------------- I logged in as donnersj. In My activity of DWP, there are following requests which throws error when tried to open it. REQ000000602441 REQ000000601766 REQ000000600974 REQ000000598350 REQ000000597376 REQ000000595637 REQ000000594763 REQ000000594825 The older approver for the above requests is Maurice Leinarts. His profile is in delete. Is this affecting the behaviour? Please investigate and fix it.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Problem: Requests in DWP/DWPC are active even if the associated incidents are close in SmartIT/ITSM 3WE What: Requests in DWP/DWPC are active even if the associated incidents are close in SmartIT/ITSM Where: Prod - DWP version 23.3.03 | build number: 5 When: Issue reported on 07/07 Extent: Requests with INC template "Cebi Incident Template" and submitted by user "Paul Elvinger" ---------------------------------------------------------------------------------------------------- Action Taken: 08/07: 1. Request 25455, 24824, 24825, 23904 are in active status even if their associated incidents INC000000016452, INC000000015931, INC000000015932, INC000000015414 are ckosed in ITSM/SmartIT. 2. All the above service requests are using template "Cebi Incident Template" to create incident and are submitted by Paul Elvinger this is common in all the affecetd requests. 3. Tried replicating the issue in QA env, strange behaviour observed. 09/07: 1. Closed the requests over a call 2. Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
+          <t>Problem: VZINC0001575726: DWP My Activity Internal Server Error when opening approval as delegate 3WE What: VZINC0001575726: DWP My Activity Internal Server Error when opening approval as delegate Where: vz-prod for a specific user donnersj When: when user donnersj tries to view REQs requested by leijkelenkamp Extent: Issue is with one user only ---------------------------------------------------------------------------------------------------- Action Taken: --&gt; 4th June: Called customer on +31 622124149, no response. --&gt; Sent an email We found that Request REQ000000602441, the Requested by user is "leijkelenkamp" and Requested For user is "leijkelenkamp" --&gt; When user/delegated approver donnersj tries to open the REQ000000602441 in DWP, they get an error. --&gt; -Reason for this error is in SRM:Request for request REQ000000602441,The user "leijkelenkamp" shows as Requested By and Requested For --&gt; -So technically user donnersj not entitled to see the request --&gt; I have confirmed with engineering that the delegate user will not be able to open the request in my/past activity. --&gt; 5th June: Called and spoke to the customer, they will check my email and update the case tomorrow --&gt; 6th June: Customer need solution for this problem applied for the entire organization. --&gt; The latest scenario is the user ? leijkelenkamp is not with the organization anymore but there are approvals in his name. Since both requested for &amp; by is leijkelenkamp , now the alternate approvers can?t view this request at all. --&gt; For the request - REQ000000602441, the alternate approver is vankanf. --&gt; 9th June: Advised that alternate approvers will not be able see the requests. If the user 'vankanf' views the REQ000000602441, he will be able to view it as the user is not an alternate approver but the main approver. --&gt; In order to approve the requests which are still pending with leijkelenkamp , you can login with leijkelenkamp credentials and approve the requests or add an approver from their User Preferences to donnersj and have donnersj approve the request. However the user donnersj will still not be able to see the REQs as they are the alternate approver and not the main approver --&gt; 10th June: Follow-up email sent --&gt; Customer Query: But I would like to have permanent solution for this scenario. The request shared was only an example. I want R&amp;D team to come up the design fix so that in future, when such scenarios are faced, system should handle it. Please discuss internally and let me know BMC?s action on this case. 11/06/2025 &gt;&gt; Below email is sent to the customer based on their queries &gt;&gt; As mentioned in Naveed?s earlier response, this appears to be an out-of-the-box behavior, and at the moment, there isn?t a supported way to modify it. &gt;&gt; To further validate, we tested this exact use case in our in-house test environment. We created "User 1" as the main approver and "User 2" as the alternate approver for "User 1". A Service Request (REQ000000000911) was then submitted and approved by "User 1". Afterward, we removed "User 1" from the CTM:People form by setting their status to "Delete". Even though "User 2" was set as the alternate approver, but was not actively involved in the approval process of (REQ000000000911), this REQ was actually approved by the main approver "User 1". As expected, (REQ000000000911) does appear in "User 2" past events, but the "User 2" is not able to access it and getting the same error as your alternate approver is getting. &gt;&gt; Given this, our suggestion would be to kindly raise an Idea. If it garners enough interest through votes, our R&amp;D team probably may consider this in a future release. &gt;&gt; Unfortunately, there are no further actions we can take in this specific scenario at the moment. I truly apologize for any inconvenience this may have caused and sincerely appreciate your understanding. &gt;&gt; Awaiting for customer to respond 13/06/2025 &gt;&gt; As customer per the customers concern we have raised a formal escalation with DWP R&amp;D Team &gt;&gt; Awaiting for their response 19/06/2025 &gt;&gt; Update received from the R&amp;D team is shared with the customer: It appears the issue may be related to the fact that the user "Maurice Leinarts" does not have a Login ID specified in the CTM:People form. Interestingly, the alternate approver configuration is set up using "leinartm" as the Login ID, but this ID isn't currently reflected in the CTM:People record. To confirm this with certainty, we would need to enable DWP Tomcat logging in DEBUG mode while attempting to access DWP as the alternate user. If this is indeed the cause, would you be open to adding the Login ID back into the CTM:People form for "Maurice Leinarts"? &gt;&gt; Awaiting for customer to respond 20/06/2025 &gt;&gt; Customer shared the details and the response is shared with the R&amp;D team &gt;&gt; I would like you to confirm that you are investigating to provide solution to fix the issue at system level but just for 1 user. Regarding your request, Maurice Leinarts profile is in delete status. Hence, he won?t have login ID. I can?t add his login ID in production for testing purpose which will in turn send wrong alarm to other monitoring systems in place. Sailpoint is also handling these user profile data. &gt;&gt; Awaiting for R&amp;D Team to respond 24/06/2025 &gt;&gt; Reviewed the logs and the logs are shared on the R&amp;D Escalation 19:03:10.181 | http-nio-9000-exec-45 | RID: d6097d32c62a41cac5134484780ee717 | OpId: 79c83e6c-5652-46b9-92b8-e3bd3b | DEBUG | c.b.b.m.service.SecurityService | Creating of AR server user objects for MyIT-ITSM 19:03:10.182 | http-nio-9000-exec-45 | RID: d6097d32c62a41cac5134484780ee717 | OpId: 79c83e6c-5652-46b9-92b8-e3bd3b | DEBUG | c.b.b.m.providers.ArServiceBase | Loading CTM person by login id 'leinartm' 19:03:10.194 | http-nio-9000-exec-45 | RID: d6097d32c62a41cac5134484780ee717 | OpId: 79c83e6c-5652-46b9-92b8-e3bd3b | DEBUG | c.b.b.m.providers.ArServiceBase | Person was not found 19:03:10.194 | http-nio-9000-exec-45 | RID: d6097d32c62a41cac5134484780ee717 | OpId: 79c83e6c-5652-46b9-92b8-e3bd3b | DEBUG | c.b.b.m.c.RequestContextImpl | Closing request... 19:03:10.194 | http-nio-9000-exec-45 | RID: d6097d32c62a41cac5134484780ee717 | OpId: 79c83e6c-5652-46b9-92b8-e3bd3b | INFO | c.b.b.m.f.r.UserPrincipalRequestWrapper | UserPrincipalRequestWrapper.getUser: donnersj 19:03:10.195 | http-nio-9000-exec-45 | RID: d6097d32c62a41cac5134484780ee717 | OpId: 79c83e6c-5652-46b9-92b8-e3bd3b | INFO | c.b.b.m.f.r.UserPrincipalRequestWrapper | principal.getName(): donnersj 19:03:10.195 | http-nio-9000-exec-45 | RID: d6097d32c62a41cac5134484780ee717 | OpId: 79c83e6c-5652-46b9-92b8-e3bd3b | INFO | c.b.b.m.f.r.UserPrincipalRequestWrapper | UserPrincipalRequestWrapper.getUser: donnersj 19:03:10.195 | http-nio-9000-exec-45 | RID: d6097d32c62a41cac5134484780ee717 | OpId: 79c83e6c-5652-46b9-92b8-e3bd3b | ERROR | c.b.b.m.r.e.ExceptionMapperProvider | jakarta.servlet.ServletException: Request processing failed: java.lang.NullPointerException: Cannot invoke "com.bmc.bsm.myit.vo.assistance.Person.getLoginId()" because "person" is null &gt;&gt; Awaiting for R&amp;D team to respond 27/06/2025 &gt;&gt; Below update is shared with the customer: &gt;&gt; Login IDs are a required element for both Digital Workplace (DWP) and Digital Workplace Catalog (DWPC). At this time, there are no plans to change this behavior based on the support use case where users do not have a login ID. For your reference, we've included helpful documentation links that explain where and why login IDs are needed. As a workaround, for specific scenarios where a login ID is not available, you may consider using Approval Central or the IS approval console. &gt;&gt; Digital Workplace Documentation: Permissions for BMC Helix Digital Workplace end users. To access BMC Helix Digital Workplace, end users require a login ID and password in BMC Helix ITSM. &gt;&gt; https://docs.bmc.com/xwiki/bin/view/Service-Management/Employee-Digital-Workplace/BMC-Helix-Digital-Workplace/dwp233/Planning/Security-planning/Roles-and-permissions/ &gt;&gt; Digital Workplace Catalog documentation: User account fields When you create user accounts, you must provide the following information: &gt;&gt; https://docs.bmc.com/xwiki/bin/view/Service-Management/Employee-Digital-Workplace/BMC-Helix-Digital-Workplace/dwp233/Administering/Administering-BMC-Helix-Digital-Workplace-Catalog/Setting-up-user-accounts-and-granting-access-to-BMC-Helix-Digital-Workplace-Catalog/Adding-users/ &gt;&gt; Awaiting for customer to respond 30/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 02/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 03/07/2025 &gt;&gt; Customer asked to keep the case on pending &gt;&gt; Awaiting for customer to respond 07/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 08/07/2025 &gt;&gt; Closing this case ---------------------------------------------------------------------------------------------------- Action Plan: Have provided solution to the customer. Waiting for their response &gt;&gt; Awaiting for customer to respond &gt;&gt; Awaiting for R&amp;D Team to respond &gt;&gt; Awaiting for customer to respond &gt;&gt; Awaiting for R&amp;D Team to respond &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Data:Investigate data sync issue between Remedy and Service Desk.:R&amp;D</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Approval:Error due to deleted approver profile; needs handling for delegate approvals.:R&amp;D</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2008425</v>
+        <v>1991552</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Unable to edit Server Service Questionary in DEV</t>
+          <t>Enhanced Catalog (DWPA) Entitlements Issue</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dear Team, We are Unable to edit Server Service Questionary in DEV. Please find the attached error screenshot.</t>
+          <t>Hello Team, We have just created a new service on DWPA called "Hardware Issues" and we have created a new entitlement for it called "Hardware Issues" to make the service visible for 4 companies including "Vodafone United Kingdom" and 1 support group as attached in the screenshot below. However, this user "pavani.gogineni1@vodafone.com" who is from "Vodafone United Kingdom" can't see the service. Moreover, the second user "Muthukumar.J2@Vodafone.com" is a member in the support group existing within the entitlement and can't see the service as well. Could you please support in this issue and clarify why the "Hardware Issues" entitlement is not reflected successfully? Thanks, Rehab</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Problem: Unable to edit questionnaire 3WE What: Customer has a questionnaire "Server", whenever end user tries to edit the questionnaire we get an error Error retrieving workflow questionnaire information Where: Dev - DWP version 25.2.00 | build number: 35 When: Issue reported on 07/07 Extent: One service affected. Steps to replicate: 1. Login to DWPC -&gt; Services -&gt; Services 2. Open service "Server" -&gt; Edit -&gt; Workflow 3. Click in Edit questionnaire, error message will pop up ---------------------------------------------------------------------------------------------------- Action Taken: 07/07: 1. R&amp;D discussion with logs and analysis: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1751895614573?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1751895614573&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1751895614573 2. Issue got resolved after removing input variable with the "Record" type from the workflow of this service 10/07: 1. Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
+          <t>Problem: Enhanced Catalog (DWPA) Entitlements Issue 3WE What: Enhanced Catalog (DWPA) Entitlements Issue Where: oneitsm-prod When: When entitlements were created Extent: Issue with one entitlement ---------------------------------------------------------------------------------------------------- Action Taken: 4th June: Sent KB 000406247 to the customer. Also advised that if the above is in place, then you can try doing Service Cache Reset during off business hours from DWP Catalog &gt;&gt; Application Settings (gear icon) &gt;&gt; Application Caches &gt;&gt; Reset Service Cache 5th June: Called customer on +20 1226154332, no response. Follow-up email sent 6th June: Called and spoke to the customer, they will get back to us on Tuesday as they are on leave 10th June: Customer to try the provided solution. 14/06/2025 &gt;&gt; I?ve reviewed the entitlements in DWP Catalog for the two users you mentioned - "pavani.gogineni1@vodafone.com and Muthukumar.J2@Vodafone.com". Upon checking entitlements in DWPC, I observed that "pavani" is currently entitled to the Hardware Issues service. However, "Muthukumar" is not entitled to the same. &gt;&gt; As you mentioned, the attributes were added by selecting the company that resolved the issue. However, when I tested this by raising a request as "Muthukumar" in the DWP end-user console, I noticed that the "Hardware Issues" service is still not entitled for him, whereas it is available for "pavani". This appears to be because "Muthukumar" belongs to the company "Vodafone India Services Private Limited", which is currently not included in the attribute configuration for the "Hardware Issues" entitlement. &gt;&gt; Awaiting for customer to respond 16/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 19/06/2025 &gt;&gt; Customer confirmed for the call and it is scheduled for tomorrow 20/06/2025 &gt;&gt; Below points were discussed on the call ? During the session, we first enabled the logs before replicating the issue for detailed analysis. ? We then reviewed the Support Group form and noted that the Support Group "Service Desk IT-EN-TSSI" is associated with the Support Company "Vodafone Service Desk Operations". ? However, we observed that the user "Muthukumar.J2@Vodafone.com" in the People form belongs to the Company "Vodafone India Service Private Limited". ? Although the user "Muthukumar.J2@Vodafone.com" is indeed a member of the Support Group "Service Desk IT-EN-TSS" but this support group is linked to Support Company "Vodafone Service Desk Operations", whereas the user is tied to "Vodafone India Service Private Limited". ? As a result, even though the Support Group is selected under the entitlement?s attributes, the entitlement will not function correctly unless the Support Group?s company aligns with the user?s company listed under the General tab in the CTM:People form. ? This is a designed behavior, the entitlement attributes reference the company details directly from the CTM:People form. &gt;&gt; Customer confirmed to close the case &gt;&gt; Closing this case ---------------------------------------------------------------------------------------------------- Action Plan: Waiting for customer's response. Solution has already been provided &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Customization:Error editing questionnaire; check customization settings.:NA</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>#PBM:DWPC:Entitlement:Check entitlement configuration for visibility issues.:Configuration</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2008565</v>
+        <v>1992812</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Digital Workplace Catalog permissions</t>
+          <t>Dev DWPC - Map to form - no data tables available</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hello, we need the following users to have administrator permissions for Digital Workplace Catalog: - DEV env: CHLE0 TULU0 ALRA0 CAPA0 VIAL0 POAN0 - QA env CHLE0 TULU0 ALRA0 CAPA0 VIAL0 POAN0 - PRD env CHLE0 TULU0 ALRA0 Thanks best regards</t>
+          <t>HI, we are not able to see the data tables when we try to map an action in any dev dwpc form. Please find the attached screenshot for reference</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Problem: Digital Workplace Catalog permissions\ 3WE What: Digital Workplace Catalog permissions Where: DWP version When: issue reported on 07/07 Extent: Few users ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; Shared the steps &gt;&gt; Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
+          <t>Problem: Dev DWPC - Map to form - no data tables available 3WE What: Dev DWPC - Map to form - no data tables available Where: nordea-dev When: when mapping data in questionnaire Extent: High ---------------------------------------------------------------------------------------------------- Action Taken: 6th June: Advised the customer to check. To fix, I did test connection for all connectors. 9th June: Customer advised to monitor for couple of days 10th June: Customer confirmed on Teams to soft-close the case. They will reopen this case or reach out to me directly if the issue reoccurs 11th June: Customer reopened the case. I did test connection on 6th June for all Connectors after which it started working, however today again they faced the same issue. Issue is not reproducible now as Manohar Machani has already done Test Connection. Customer would like to get to the root cause as the issue reoccurred after 5 days. Checked DWP master and slave pods were restarted 140 days ago. Reset Service Cache was done on 2nd June. Need further assistance from R&amp;D to identify why the issue is intermittent Escalated to R&amp;D for further assistance 12th June: Restarted platform user pod. Waiting for customer to test 13th June: Customer advised to leave the case open for few days 16/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 19/06/2025 &gt;&gt; Closure received &gt;&gt; Closing the case ---------------------------------------------------------------------------------------------------- Action Plan: Customer advised to leave the case open for few days &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:Permissions:Granted administrator permissions to specified users.:Customization</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>#PBM:DWPC:Data:Data tables not visible in form mapping; investigate configuration.:NA</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2009315</v>
+        <v>1993411</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Automating creation of user accounts in Helix ITSM vs. DWP</t>
+          <t>States not updated</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>I have an outstanding recommendation from the Vodafone Security Team to implement automatic user creation in VNIPM from Active Directory data held in an internal Vodafone User Access Management (UAM / WIAM) for all members of the Vodafone Network Operations division. All users would require a basic level of access with Read-Only permissions and Incident Submit. We would like these users to be able to access both Classic Mid-Tier UI and SmartIT (which has previously caused us issues due to some customizations). However, I now have a related requirement to be able to give all users access to only VNIPM DWP regardless of whether they already have a VNIPM Helix ITSM account or not. Questions: 1. Is it possible to give users access to DWP only? 2. Is it possible to automate this from an external source? I.e. to be driven by the external source via an API.</t>
+          <t>Hi, Even though the requests have been approved, the status in Catalog is ?Awaiting Approval?. If you search for any of the requests in the WOI:WorkOrder form, you will find the WOs created. A more detailed document is attached. The failed requests are: 256374 253372 251598 250090 249343 246390 246814 247311 248461 247311 248461 245002 248463 Could you please check why the status of the requests has not been updated in the Catalog? Regards.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Problem: 3WE What: Where: When: Extent: ---------------------------------------------------------------------------------------------------- Action Taken: ---------------------------------------------------------------------------------------------------- Action Plan: ---------------------------------------------------------------------------------------------------- Action Owner:</t>
+          <t>Problem: Status not getting updated. 3WE What: Requests have been approved, the status in Catalog is ?Awaiting Approval?. If you search for any of the requests in the WOI:WorkOrder form, you will find the WOs created. Where: Prod - DWP version 25.1.01 When: Issue reported on Extent: 09/06 ---------------------------------------------------------------------------------------------------- Action Taken: 09/06: "Can we replicate the issue on demand? If yes, can you provide us some available time slots for a teams call? " 11/06: - Followed up 12/06: - Followed up 13/06: - Customer trying to replicate the issue. 16/06: - Followed up - Refer to the my bookmarked mail for customer's latest response. 19/06/2025 &gt;&gt; Below update is shared with the customer &gt;&gt; Upon reviewing Request ID: 253856 in the SB:ServiceRequestStub form, I can see that it appears to be approved, and the transmission status shows as sent for both approvals. Based on this, the request should ideally be in an approved status rather than waiting for approval. &gt;&gt; However, after reviewing the error details for this request ID, here?s what I?ve observed: &gt;&gt; com.bmc.myservice.common.util.exception.MyServiceNotFoundException: [ERROR (302): This record does not exist or you do not have permissions to access this record.] &gt;&gt; Caused by: ERROR (302): Entry does not exist in database &gt;&gt; This is coming from: com.bmc.arsys.server.rx.services.process.ProcessServiceImpl.updateProcessContextWithStatusCompleted &gt;&gt; From my understanding, this suggests that the system attempted to mark a process instance as completed, but the required record was missing, possibly an associated approval-related entry. &gt;&gt; To further investigate this issue, we would need to capture the following logs in Debug mode: -- API / SQL / FLTR -- Process logs -- MyIT-SB logs &gt;&gt; Capturing these logs during the issue replication will help us get a clearer picture of the root cause. If this issue is replicable on demand, we?d be happy to connect on a quick call to capture the necessary logs in real-time. Please let us know if that?s feasible from your end. &gt;&gt; In parallel, I?m also checking this with our R&amp;D team and will keep you posted if there are any updates or insights from their side. &gt;&gt; Awaiting for customer to respond 23/06/2025 &gt;&gt; Customer shared the details with us: One of the cases created was 166953 in which it is seen that the request is approved but does not generate the corresponding WO. Also 2 other requests have been created so that they can test: 166954 and 166955. We remind you that the forms for testing are: | SB:ServiceRequestStub | AP:Detail-Signature &gt;&gt; Upon reviewing the DWPC Service Catalog "NEW HARDWARE", we identified a condition error in the associated Workflow "GLOBAL_COS_HW", specifically after the "Approval UCL BR, Approval UCL USA and Approval UCL ES" call activity. The word "Approved" was misspelled in the condition as "Aproved", which was the cause of the issue. Please find the screenshot below for your reference. &gt;&gt; I?ve now corrected the spelling within the condition and saved the changes. You can see the updated screenshot below as well. &gt;&gt; After making this adjustment, I tested by approving the DWPC Request (166954), this successfully created the corresponding Work Order (WO0000000117003) and also generated the expected entry in the SB:ServiceRequestStub form. &gt;&gt; Based on my testing on the QA instance (as per your instructions), everything appears to be working smoothly now, and the issue seems to be resolved. &gt;&gt; Awaiting for customer to respond 26/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond. &gt;&gt; Customer responded: Whether the changes are made on the Prod as well. &gt;&gt; To which we have responded that we did not made changes on Prod. 27/06/2025 &gt;&gt; Customer responded with more details in regards to the issue on Prod: -- I asked if in the PRO environment the modifications had been made, as I have not seen the error (the word APROVED) discussed in the previous messages. Thank you very much for the help but rechecking the ids of the requests that were provided when opening this case and, unlike the error that was reproduced in the QA environment, most of the requests were approved but did not generate the corresponding WO. The original listing is as follows: 256374 | 253372 | 251598 | 250090 | 249343 | 246390 | 246814 | 247311 | 248461 | 247311 | 247311 | 248461 | 245002 | 248463 | -- Each case is detailed below: 256374: generated ticket 253372: generated ticket 251598: appears approved but has not generated the corresponding WO and in DWPC it appears as closed. 250090: appears approved but has not generated the corresponding WO and in DWPC it appears as closed. 249343: appears approved but has not generated the corresponding WO and in DWPC it appears as closed. 246390: the states in DWPC do not coincide with those that appear in the SB:ServiceRequestStub form. 246814: the states in DWPC do not coincide with those that appear in the SB:ServiceRequestStub form. 247311: the states in DWPC do not coincide with those that appear in the SB:ServiceRequestStub form. 248461: appears approved but has not generated the corresponding WO and in DWPC it appears as closed. 247311: the states in DWPC do not coincide with those that appear in the SB:ServiceRequestStub form. 248461: appears approved but has not generated the corresponding WO and in DWPC it appears as closed. 245002: the states in DWPC do not coincide with those that appear in the SB:ServiceRequestStub form. 248463: appears approved but has not generated the corresponding WO and in DWPC it appears as closed. -- Could you please review what may have caused the states not to be reflected in DWPC and, in the cases that were approved, why the corresponding WO was not generated? -- Is there any way that states are forced to travel? And, in the cases that were approved, could the WO be generated? &gt;&gt; Need to investigate this further 30/06/2025 &gt;&gt; Followed up with the customer 01/07/2025 &gt;&gt; Investigated the request IDs shared, below findings are shared with the customer &gt;&gt; Based on the Request IDs and details you?ve kindly shared, I?ve reviewed each of them in detail. While some of the highlighted requests are over two months old and unfortunately lack historical logs?which limits our ability to fully trace the issue?we were still able to gather valuable insights by analyzing data from the IS side, ITSM, and the Process Viewer. &gt;&gt; Below, I?ve outlined my observations against each of the request IDs for your convenience: &gt;&gt; Request ID	Your Comment	My Observation &gt;&gt; 256374	generated ticket	Flow looks good?no issue observed. &gt;&gt; 253372	generated ticket	Flow looks good?no issue observed. &gt;&gt; 251598	appears approved but has not generated the corresponding WO; appears as closed in DWPC	In the Process Viewer, the approval timed out after 2 months and failed. Instead of flowing to the Create Work Order step, it went to Activity Logs ? UCL Rejected (see Screenshot 1). The "Approval UCL US" call activity is using SB_UCL_USA, which triggers the Request Approval workflow. The process seems to have stalled at the Receive Task, which has a 2-month timer. Since it didn?t progress, the task timed out, and the process failed. Only two approval-related entries exist in the External Activity table, confirming it never moved forward. &gt;&gt; 250090	same as above	Same observation as request ID 251598. &gt;&gt; 249343	same as above	Same observation as request ID 251598 and 250090. &gt;&gt; 246390	state mismatch between DWPC and SB:ServiceRequestStub	The Manager Approval (using "SB Request Manager Approval") passed successfully. However, the second approval ("Approval UCL US") triggered SB_UCL_USA and failed due to timeout after being stuck at the Receive Task. The status was sent correctly from SB:ServiceRequestStub but was not synced at DWPC, possibly due to a polling delay. Manually syncing the status via the IS:External Activity table should resolve this. &gt;&gt; 246814	same as above	Same observation as request ID 246390. &gt;&gt; 247311	same as above	Same observation as request ID 246390 and 246814. &gt;&gt; 248461	same as 251598	Same observation as request ID 251598, 250090, and 249343. &gt;&gt; 245002	state mismatch	Same observation as request ID 246390, 246814, and 247311. &gt;&gt; 248463	same as 251598	Same observation as request ID 251598, 250090, 249343, and 248461. &gt;&gt; Awaiting for customer to respond 03/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond &gt;&gt; Customer requested for screenshot, attached the screenshot and shared with the customer &gt;&gt; Awaiting for customer to respond &gt;&gt; Customer had a follow up query: Could you please tell me in which form is the IS:External Activity table indicated for Request ID 246390? &gt;&gt; We have shared below update on this: &gt;&gt; Kindly refer to the following two forms within the Innovation Studio for the details: myit-sb:ExternalActivity | myit-sb:ServiceRequest &gt;&gt; If you have any further queries or would like to walk through this together, I?d be more than happy to hop on a quick Teams call at your convenience. 04/07/2025 &gt;&gt; Followed up with the customer over the case | Tried calling but there was glitch in the audio, hence emailed over the case &gt;&gt; Awaiting for customer to respond 07/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 08/07/2025 &gt;&gt; Got closure on this case &gt;&gt; Closing this case ---------------------------------------------------------------------------------------------------- Action Plan: Need to investigate further &gt;&gt; Awaiting for customer to respond &gt;&gt; Need to investigate this further &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Integration:Guide on automating user access via API.:Educate</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Approval:Investigate why approval status not updated in Catalog.:R&amp;D</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2009298</v>
+        <v>1993547</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Issue while raising DWP Service Request from Chatbot/HelixGPT</t>
+          <t>Upgrade to 23.3.04 patch</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Outlook Access Request is published in HelixGPT. Customer's requirement is that they want the Date in DD/MM/YYYY Format. However, after changing the prompt to accept the Date in DD/MM/YYYY format, the Service Request creation fails. The reason is that DWP always accepts the Date in MM/DD/YYYY format. NOTE: When we look at the Service, the Customer is seeing the Date in DD/MM/YYYY format, while when checking from the BMC end, It shows in MM/DD/YYYY Kindly help check with the DWP R&amp;D if this is expected behavior, as the Date format in the question seems to be changing depending on the Country/Region and is not consistent. If required, kindly engage the HelixGPT Team as well.</t>
+          <t>Hi Team, we had requested to upgrade DEV to 23.3.04. Things seems to be working fine. Please deploy the same patch in QA. However make sure no Sample Data, Additional DWPC Catalogs, DWP Studio pages are deployed as part of patch. Just the patch upgrade and no sample data.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Problem: Issue while raising DWP Service Request from Chatbot/HelixGPT 3WE What: Issue while raising DWP Service Request from Chatbot/HelixGPT Where: HelixGPT Manager When: When submitting DWP request from HelixGPT Extent: Issue with date format ---------------------------------------------------------------------------------------------------- Action Taken: 9th July: Initiated backline chat: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1752075455846?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1752075455846&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1752075455846 10th July: Updated date format in COPS to Updated the Date format to DD/MM/YYYY HH:MM:SS (24-hour) in COPS as advised by Sumeet Das however issue still persists. Based on discussion with R&amp;D, reached out to Kalpana on Teams asking if we can get on a call. She advised to get in touch with VijayKumar Rodge. 11th July: Got on a call with VijayKumar Rodge to understand the issue as follows: Customer has an SR called Outlook Access that has a question field called "AccessDate" which is in mm/dd/yyyy however this date format depends on the system settings. In HelixGPT Manager they have modified a prompt for v2 (Active) where the date format should be DD/MM/YYYY however when they submit the request using HelixGPT, it fails with error: Your request is submitted and processed. Here's the status: COMPLETED result: Error. The date conversion is not working. Customer should see it in DD/MM/YYYY format. The one that is going in payload is yyyy/dd/mm Updated the Date format to DD/MM/YYYY HH:MM:SS (24-hour) in COPS as advised by Sumeet Das. Customer has tried changing the prompt in IS&gt;&gt;HelixGPT Manager&gt;&gt;For v2 )Active). Earlier it was yyyy/dd/mm which is what is getting pulled in Network Paylod (Dev tools) Took screenshots of the issue and escalated to R&amp;D. 14/07: 1. Customer and R&amp;D call: https://bmcsoftware-my.sharepoint.com/:v:/g/personal/achabuks_bmc_com/EXegH6poI0xMhZh-TaNGRAEBYbPKkeVZZXLdfcBueJRaWA?e=cH1dH4&amp;nav=eyJyZWZlcnJhbEluZm8iOnsicmVmZXJyYWxBcHAiOiJTdHJlYW1XZWJBcHAiLCJyZWZlcnJhbFZpZXciOiJTaGFyZURpYWxvZy1MaW5rIiwicmVmZXJyYWxBcHBQbGF0Zm9ybSI6IldlYiIsInJlZmVycmFsTW9kZSI6InZpZXcifX0%3D ---------------------------------------------------------------------------------------------------- Action Plan: Need to schedule an internal call with VijayKumar Rodge , Aparna Nevase, Rajni Patil and DWP R&amp;D to check if the issue can be fixed ---------------------------------------------------------------------------------------------------- Action Owner: DWP Engineering</t>
+          <t>Problem: Upgrade to 23.3.04 patch 3WE What: Upgrade to 23.3.04 patch Where: closebrothers-qa When: customer would like to upgrade Extent: Upgrade request ---------------------------------------------------------------------------------------------------- Action Taken: 9th June: Raised CRQ000001693139 . It has been scheduled for 11th June 13th June: Follow-up email sent to the customer to take necessary action on CRQ000001693139 16th June: CRQ000001693139 has been scheduled as follows: Change Summary: Upgrade to 23.3.04 latest patch-closebrothers-qa Scheduled Start Date: 6/17/2025 4:00:00 PM UTC Scheduled End Date: 6/18/2025 4:00:00 PM UTC 19/06/2025 &gt;&gt; Change request is complete and informed the customer &gt;&gt; Awaiting for customer to respond 23/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 27/06/2025 &gt;&gt; No pending action, hence closing this case ---------------------------------------------------------------------------------------------------- Action Plan: Waiting for CRQ000001693139 to be implemented &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Defect:Date format inconsistency in DWP; engage R&amp;D for fix.:R&amp;D</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Upgrade:Upgrade patch applied to QA without sample data.:NA</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2009757</v>
+        <v>1993565</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DWP requests can't be cancelled</t>
+          <t>DWP Request Comment Not Reflecting in ITSM/Smart IT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hi Support, I've created an entry using DWP for the Incident Management backend. The submission is OK but then I've tried to cancel the request by clicking "cancel". This operation never gets completed as the message "the action is taking longer than expected but eventually will get completed" appears. If've waited for more than 5 mins and neither the backend entry nor the frontend reflects the change, even when clicking again in CANCEL. See screenshots for details. Please, review. Vanessa</t>
+          <t>Hi Team, Comments from DWP are not reflecting as the worklog activity in ITSM/Smart IT. This issue is randomly experienced in some requests (Incidents and work orders) in production environment. Please find some requests below having this issue. Tickets with this issue for your reference - 1365190 1282195 1330361 Could you please share the root cause of this issue and help in resolving it at the earliest. Thank you!</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Problem: 3WE What: Where: When: Extent: ---------------------------------------------------------------------------------------------------- Action Taken: ---------------------------------------------------------------------------------------------------- Action Plan: ---------------------------------------------------------------------------------------------------- Action Owner:</t>
+          <t>Problem: Comments from DWP not reflecting in SmartIT/ITSM 3WE What: Customer reported that comments from DWP are not reflecting in associated fulfilment (Incident/Workorder) intermittently. Where: Prod - DWP version 25.1.00 When: Happening intermittently - latest request 2nd June Extent: Intermittent ---------------------------------------------------------------------------------------------------- Action Taken: 09/06; 1. Checked all the points mentioned in the KA: 000402812 (https://bmcapps.lightning.force.com/lightning/r/Knowledge__kav/ka3cx0000005rRtAAI/view) 2. R&amp;D discussion: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1749475897196?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1749475897196&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1749475897196 10/06; 1. Escalated the case to R&amp;D: https://jira.bmc.com/browse/DRIIT-79094 13/06: 1. For the existing service request 1365190 we can try to replay test message with enabled logs by manipulating catalog database tables and see if issue reproduces. Let me know if we can do that. 2. Customer response: Could you please share the complete details of how are you planning to execute it, along with the steps involved? 16/06: 1. we can take information from QueueTaskHistory and copy it to QueueTask so it will replay sending comment, or we can just add new comment to existing request and capture logs. 2. Informed the customer, waiting for their response if we can move forward 18 Jun: Customer wants to hold this case and troubleshoot the issue after 24th June. 9 July: Processed request from QueueTask from and tried to capture the logs but that didn't helped us, so we may need to have a call with customer and capture the logs. 18/07/2025 &gt;&gt; Had a discussion on the US R&amp;D Swarm call and below is the update shared with the customer &gt;&gt; Kindly note, if the DWPC Service Requests are already marked as Completed or Closed, it is not possible to process the QueueTaskHistory and copy it to QueueTask. For the comment transaction to be processed successfully, both the Fulfillment Ticket and the DWPC Service Request must remain in an active state. &gt;&gt; Once a request is completed/closed, the associated queuetaskhistory cannot copied to queuetask. &gt;&gt; To better understand and analyze this use case, logs will be required. However, since this behavior is not currently reproducible, it is difficult to pinpoint the exact cause on this issue. &gt;&gt; Awaiting for customer to respond 21/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 22/07/2025 &gt;&gt; Customer agreed to close the case &gt;&gt; Closing this case ---------------------------------------------------------------------------------------------------- Action Plan: Waiting for customer's response 10 July: Need to have a call with customer and capture logs and the logs capture by processing records in QueueTask and QueueTaskHistory by following the KA 000421124 dose not help. &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Request:Investigate request cancellation delay issue.:R&amp;D</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Integration:Investigate DWP-ITSM comment sync issue.:R&amp;D</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2009756</v>
+        <v>1993836</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DWP Service issue</t>
+          <t>DWP - Notification Template Changes</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hello BMC, We are facing the following problem, that is happening only in our client?s DEV environment. The attached DWP Service called ?Nuova Change Request? has a very simple workflow: ?	Approval to a specific user; ?	Change Request creation. Once submitted, the DWP request immediately reaches the ?In Progress? state instead of the ?Approval? state. After a lot of time (more or less 20 minutes), the approver sees the request in his DWP. (see attachment 1)  If he tries to approve, nothing changes. More precisely: ?	We cannot find the DWP request in Helix ITSM; ?	We do not see any Change Request getting created; ?	System is not throwing any error. (see attachment 2) We expect instead that the request stays on ?Approval? state and after the approval of the user, we expect the Change to be created (this is correctly happening in another instance of another client). For any answer, please involve also patrick.caprioli@alten.it, alessandro.vitagliano@alten.it and andrea.polverino@alten.it . Many thanks in advance.</t>
+          <t>Hi Team, We've modified the email template for end-user notifications when a request is submitted, but the changes aren't effective. We added the service request ID in header. PFA. If we use the Sample Notification button, we do see the change. Can you check? Regards, Rocio</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Problem: Delay of status transmission of request 3WE What: Delay of status transmission of request Where: Dev - DWP version 25.1.01 and Build number 11 When: Issue reported on 09 Extent: Performance ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; Collected apifiltersql, myit-sb logs for request 13 and CRQ000000000616 &gt;&gt; R&amp;D escalation: https://jira.bmc.com/browse/DRIIT-79715 &gt;&gt; Pod restart resolved the issue &gt;&gt; Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
+          <t>Problem: Notification Template Change 3WE What: modified the email template for end-user notifications when a request is submitted, but the changes aren't effective. We added the service request ID in header. PFA. If we use the Sample Notification button, we do see the change. Where: DWP-Notification When: Notification Modification Extent: New change ---------------------------------------------------------------------------------------------------- Action Taken: Checking if restart is needed Pods were fine and did not get anything in logs. Customer to confirm. To set up call next week with customer and replicate the issue and capture logs 23/06/2025 &gt;&gt; Followed up with the customer for the teams call &gt;&gt; Awaiting for customer to respond 25/06/2025 &gt;&gt; Had a call with the customer and configuration looks good in terms of changes customer did in the Heading of the Notification email template, but the changes aren't reflecting. Also, we suggested for a DWP Pods restart over Off business hours. 27/06/2025 &gt;&gt; Followed up with the customer that we will perform the restart activity post 9 PM Spanish Time &gt;&gt; Restart was performed on the scheduled timeline 30/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 03/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond &gt;&gt; Customer responded as below: &gt;&gt; After discussing it with the client, they requested that this information be included in the email subject, rather than the heading. Please close the case because we'll make the change to the notifications when we upgrade. 04/07/2025 &gt;&gt; We informed the customer that we will close the case and shared below update with the customer &gt;&gt; As you kindly mentioned that you plan to implement notification template changes after the version upgrade, I?m assuming this would be to version 23.3.04 or 25.x. Starting from version 23.3.04, the new Helix Platform Notification Engine has been introduced, which offers enhanced flexibility and allows customization of email templates as per your preferences. For your convenience, I?m sharing the documentation link below, which provides clear and helpful guidance on setting up and leveraging this feature: &gt;&gt; https://docs.bmc.com/xwiki/bin/view/Service-Management/Employee-Digital-Workplace/BMC-Helix-Digital-Workplace/dwp251/Administering/Administering-BMC-Helix-Digital-Workplace/Leveraging-the-notification-engine-on-BMC-Helix-Innovation-Suite-for-greater-flexibility/ &gt;&gt; Closure email is sent &gt;&gt; Closing this case today EOD ---------------------------------------------------------------------------------------------------- Action Plan: R&amp;D to confirm Check if anything in logs. If all fine, restart the dwp pods once and check &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Workflow:Investigate workflow approval delay and request creation issue.:R&amp;D</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Notification Template:Check template activation and cache refresh.:Customization</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2009770</v>
+        <v>1994474</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Migrating SRM:Request to myit_sb:Servicerequest for Helix Dashboard reports</t>
+          <t>Double quotation mark in DWP-Request field causes DWP error</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dear Team, I am migrating reports from Smart Reporting to BMC Helix Dashboards. Now, I have some "old" SRM Reports to migrating . I know SRM:Request and myit-sb:Servicerequest are different forms but they are dealing with similar data. For Example, Here is the SQL request from SR : SELECT DISTINCT  YEAR(`SRM:Request`.`Completion Date`) AS C1,  `SRM:Request`.`Status` AS C2,  `SRD:ServiceRequestDefinition`.`SRD_Title` AS C3,  COUNT(DISTINCT(`SRM:Request`.`Request Number`)) FROM `AR System Schema`.`SRM:Request` LEFT OUTER JOIN `AR System Schema`.`SRD:MultipleQuestionResponse` ON (  `SRM:Request`.`InstanceId` = `SRD:MultipleQuestionResponse`.`SRInstanceID` ) LEFT OUTER JOIN `AR System Schema`.`SRD:ServiceRequestDefinition` ON (  `SRM:Request`.`SRDInstanceID` = `SRD:ServiceRequestDefinition`.`InstanceId` ) WHERE (  `SRD:ServiceRequestDefinition`.`SRD_Title` IN ('Administration et aide sur la plateforme ITSM (hors incidents)', 'Amélioration des processus et services', 'Choix de l''outil pour une nouvelle visualisation OCSIN', 'Évolution Outillage Processus pour la Gestion Opérationnelle de Services', 'Création, modification ou désactivation de Groupes de support dans ITSM', 'Correction du référentiel ITSM - CMDS')  AND `SRM:Request`.`Category 2` IS NOT NULL  AND `SRD:MultipleQuestionResponse`.`Answer In Char` LIKE '%incident%'  AND (  `SRM:Request`.`Completion Date` BETWEEN '01/01/2025 12:00:00 AM' AND '07/09/2025 08:59:30 AM'  OR `SRM:Request`.`Completion Date` BETWEEN '01/01/2024 12:00:00 AM' AND '12/31/2024 11:59:59 PM'  OR `SRM:Request`.`Completion Date` IS NULL  ) ) GROUP BY YEAR(`SRM:Request`.`Completion Date`),  `SRD:ServiceRequestDefinition`.`SRD_Title`,  `SRM:Request`.`Status` According to this idea, : https://community.bmc.com/s/idea/0873n000000TlIHAA0/detail, the "Completed date" is not added yet on myit-sb:ServiceRequest. Is there an alternative to get it in another myit-sb forms, please? It is the same problem with SRD_Title. I may have found a way by using the "processname" columns on myit-sb:ServiceRequest but is there a simpler way to select it, please? Thank you for your help in advance. I am sorry but I don't know whether I selected the right component for this ticket. Regards, Charles</t>
+          <t>On 13.03.2025 we noticed a technical error in DWP request 357636. This DWP request calls the application ?Happy? in the business service regular form BMC.CORE:BMC_BusinessService (the exact name is: 'Complaint management system ?Happy? - PROD'). The double quotes are an integral part of the name, but unfortunately are causeing this error in the DWP workflow: AR: ERROR (4558): Qualification line error; [at posttion 39, 'Name' = "Beschwerdemanagement-System "Happy" - PROD" AND 'DatasetId' = "BMC.Asset" ] Our question: Is there any way that the DWP framework can mask the double quotes WITHOUT an additional check routine to be created by us, so that these orders can be created without errors?</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Problem: According to this idea, : https://community.bmc.com/s/idea/0873n000000TlIHAA0/detail, the "Completed date" is not added yet on myit-sb:ServiceRequest. And the customer would like to confirm if there is an alternative to get completed date from another myit-sb forms. 3WE What: According to this idea, : https://community.bmc.com/s/idea/0873n000000TlIHAA0/detail, the "Completed date" is not added yet on myit-sb:ServiceRequest. And the customer would like to confirm if there is an alternative to get completed date from another myit-sb forms. Where: PROD When: Trying to migrate service requests from SRM to DWPC. Extent: ---------------------------------------------------------------------------------------------------- Action Taken: Customer has migrated the service requests from SRM to DWPC According to this idea, : https://community.bmc.com/s/idea/0873n000000TlIHAA0/detail, the "Completed date" is not added yet on myit-sb:ServiceRequest. And they would like to confirm if there is an alternative to get completed date from another myit-sb forms. It is the same problem with SRD_Title. They have found a way by using the "processname" columns on myit-sb:ServiceRequest but would like to confirm if there a simpler way to select it? 09/07: 1. R&amp;D discussion: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1752069372840?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1752069372840&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1752069372840 11/07: 1 Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: BMC</t>
+          <t>Problem: Double quotation mark in DWP-Request field causes DWP error 3WE What: noticed a technical error in DWP request 357636. This DWP request calls the application ?Happy? in the business service regular form BMC.CORE:BMC_BusinessService (the exact name is: 'Complaint management system ?Happy? - PROD'). The double quotes are an integral part of the name, but unfortunately are causeing this error in the DWP workflow: AR: ERROR (4558): Qualification line error; [at posttion 39, 'Name' = "Beschwerdemanagement-System "Happy" - PROD" AND 'DatasetId' = "BMC.Asset" ] Our question: Is there any way that the DWP framework can mask the double quotes WITHOUT an additional check routine to be created by us, so that these orders can be created without errors? Where: DWPC - Workflow When: New design Extent: Only when quotation is used ---------------------------------------------------------------------------------------------------- Action Taken: Escalation created as discussed with Daria The DWP request 357636 shared is a very old one with limited logs available. It's not helping in identifying the root cause of the issue. Can you reproduce the issue and collect the latest myit-sb, apisqlfilter, and process logs Issue recording; https://bmcsoftware-my.sharepoint.com/personal/npadhi_bmc_com/Documents/Recordings/Case%2001994474%20Double%20quotation%20mark%20in%20DWP-Request%20field%20causes-20250616_133112-Meeting%20Recording.mp4?web=1&amp;referrer=Teams.TEAMS-ELECTRON&amp;referrerScenario=RecapOpenInStreamButton.view.71af44f0-97f2-465b-8631-2448344ab4e4 Connected on Call and replicated issues. Captured and downloaded logs. Logs attached to escalation R&amp;D to check further 18/06/2025 &gt;&gt; Update received from the R&amp;D Team and below information is shared with the customer -- It is breaking in the hwf_CreateDkbWorkorderWithService workflow in the 'Get Asset / BS-Data' brick when querying the form data: -- formName=BMC.CORE:BMC_BusinessService, query='Name' = "Beschwerdemanagement-System "Happy" - PROD" AND 'DatasetId' = "BMC.Asset" -- The recommendation is to escape the double quote before passing it to the query. -- Replace the double quote with 2 double quotes. so the search string will be: 'Name' = "Beschwerdemanagement-System ""Happy"" - PROD" -- You can try this first directly on the BMC.CORE:BMC_BusinessService form - Advanced search. &gt;&gt; Awaiting for customer to respond 23/06/2025 &gt;&gt; Customer requested for the detailed steps and same is shared on the R&amp;D escalation &gt;&gt; Awaiting for R&amp;D team to respond 25/06/2025 &gt;&gt; Update received from the R&amp;D team and below info is shared with the customer &gt;&gt; Kindly use a Replace brick to substitute a double quote (") with two double quotes (""). Please refer to the screenshot below for clarity. &gt;&gt; Once that?s done, you can use the output of this brick in the Get Entry By Query brick, as shown below: &gt;&gt; ?(("'Name' = """ + ${processContext.Processed Business Service}) + """ AND 'DatasetId' = ""BMC.Asset""")?? &gt;&gt; Awaiting for customer to respond 27/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 30/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 04/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 07/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 08/07/2025 &gt;&gt; Customer agreed to close the case &gt;&gt; Closing this case ---------------------------------------------------------------------------------------------------- Action Plan: R&amp;D to suggest further Customer to confirm R&amp;D to check further and confirm. &gt;&gt; Awaiting for customer to respond &gt;&gt; Awaiting for R&amp;D team to respond &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>#PBM:SRM:Report:Guide on mapping SRM fields to Helix Dashboard.:Educate</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Workflow:Double quotes in names cause workflow errors; needs masking solution.:R&amp;D</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2009785</v>
+        <v>1995328</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Need help with data decryption on DWPC Service</t>
+          <t>Different logo for Email Template and DWP Portal</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hi Team, Good Day...! We are working on DWPC Service where we have credentials. Can you please let me know if there is capability where we can encrypt and decrypt credentials to maintain confidentiality of credentials. Thanks, Bhavesh</t>
+          <t>Hello Team, Please be informed in DWP we have requirement to have a different branding logo for DWP Email Template and DWP Portal. Please confirm on the possibility and also share if there's any article related. Hereby attaching snip for your reference. Regards, Akash</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Problem: Data decryption on DWPC Service 3WE What: Data decryption on DWPC Service Where: DWP version 25.1.01 When: Generla query Extent: Generla query ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; R&amp;D: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1752228847216?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1752228847216&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1752228847216 &gt;&gt; do not think we provide such capabilities OOTB. However, customer can make it using InnovationStudio capabilities (custom app) or delegate it to 3rd party app, or anything like that &gt;&gt; Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
+          <t>Problem: Different branding logo for DWP Email Template 3WE What: Different branding logo for DWP Email Template Where: DWP version 23.3.04 - all envs When: Query asked on 11/06 Extent: Notification template Steps to replicate: 1. Login to ITSM -&gt; CTM:People (add valid email address to your user profile and change company to BBC) 2. Login to DWP -&gt; Search and open service "Microsoft Visio Plan 2" 3. Fill the questionnaire and submit request 4. Wait for request submission email 5. Look at the email header icon, they want to have a different icon there ---------------------------------------------------------------------------------------------------- Action Taken: 12/06: 1. Refer to my bookmarked mail for solution to both queries. 13/06: 1. Followed up with the customer 17/06: 1. Customer call recording: https://bmcsoftware-my.sharepoint.com/:v:/g/personal/achabuks_bmc_com/Edsy8SOwBOFFvEo-3gmLPjoB9J6bkzgebTU-52GAmF47Dw?e=QDGIba - Informed customer to use Helix platform as email engine. - Customer wants to have a different logo for email template 18/06: 1. Asked the customer to share the icon, he wants to have in email template 2. R&amp;D discussion: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1750238774884?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1750238774884&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1750238774884 21/06/2025 &gt;&gt; Below update is shared with the customer &gt;&gt; Under the standard rebranding functionality, the logo you configure will appear both on the DWP portal and within the email template, they remain the same by default. -- Since you're currently on version 23.3.04, you have two available notification engines: ? DWP Notification Engine (the default one you're currently using) ? Helix Platform Notification Engine, which allows you to customize the email template. &gt;&gt; With the Helix Platform Notification Engine, you can indeed edit the email templates and apply a separate logo specifically for email notifications. But, if the customization of the email template goes wrong it can damage the HTML code specific to the template that is being customized. &gt;&gt; Just to confirm, since you're currently using the default DWP Notification Engine, if you wish to continue using the default engine, the logo applied through rebranding will automatically appear in both places and cannot be customized separately for email notifications. In case you switch to the Helix Platform Notification Engine then you will be able to customize the logo by customizing the HTML template. 26/06/2025 &gt;&gt; As previously mentioned, I see that you are currently on version 23.3.04 and using the default DWP Notification Engine. With this version, a new option, the Helix Platform Notification Engine, has also been introduced, offering additional flexibility. &gt;&gt; Currently, since you are using the default DWP Notification Engine, incorporating a logo can only be achieved via the Rebranding functionality. This means that the logo applied through rebranding will appear both on the DWP portal and in email notifications. Unfortunately, it is not possible to set separate logos for the portal and the email notifications when using the default DWP Notification engine. &gt;&gt; However, the newly introduced Helix Platform Notification Engine in version 23.3.04 offers greater customization. This engine supports custom templates, configured at the Innovation Suite (IS) level, which allow you to personalize the layout and even incorporate a distinct logo of your choice into the email templates. &gt;&gt; That said, please keep in mind that customizing these templates requires care, as incorrect changes may affect the HTML structure of the notification. While customization falls outside standard support, you're welcome to handle it internally or consult Professional Services (PS) for assistance. &gt;&gt; Additionally, for your convenience, please refer to the detailed documentation on the Helix Platform Notification Engine here: &gt;&gt; https://docs.bmc.com/xwiki/bin/view/Service-Management/Employee-Digital-Workplace/BMC-Helix-Digital-Workplace/dwp251/Administering/Administering-BMC-Helix-Digital-Workplace/Leveraging-the-notification-engine-on-BMC-Helix-Innovation-Suite-for-greater-flexibility/ &gt;&gt; Once you enable the new Notification Engine by following the steps mentioned in the above KA, you can proceed with customizing the templates using the steps below. However, as previously mentioned, please note that incorrect changes may affect the entire HTML structure of the template. Therefore, we kindly recommend considering support from our Professional Services (PS) team for a safe and guided customization experience. -- Modifying of notification engine email templates &gt;&gt; Notification Engine email templates should be modified using Innovation Studio Workspace. Please don't use "Manage Templates" page for editing of notification engine email templates. At first it is needed to get template id from "NotificationTemplate" record definition and then it will be used to find needed record in "TemplateMessage" record definition. Do following steps for editing templates: ? Go to IS. ? Click on Libraries then click on "Notification Service". ? Near "NotificationTemplate" click on checkbox then click on "Edit data". ? Click on Filter ? Write required name of template into field "Template Name". ? Press enter and click on "Apply filters". ? Click on record and copy value of field "ID". This is Template ID. It will be used in further steps ? Click on Close button. ? Near "TemplateMessage" click on checkbox then click on "Edit data". ? Click on Filter and write Template ID into field "Template Id" and write "body" into field "Message type". After that 31 records will be shown(one record per one locale). ? Click on record for some locale and copy value of field "Message" into some HTML editor. ? Make needed changes in HTML code. ? Then copy changes into field "Message". ? Click "Save" -- Reverting back of notification engine email templates to original. -- To revert back template to original it is needed to have the backup of original HTML template. Do following steps for reverting back of notification engine email templates to original: ? Go to IS. ? Click on Libraries then click on "Notification Service". ? Near "NotificationTemplate" click on checkbox then click on "Edit data". ? Click on Filter ? Write required name of template into field "Template Name". ? Press enter and click on "Apply filters". ? Click on record and copy value of field "ID". This is Template ID. It will be used in further steps ? Click on Close button. ? Near "TemplateMessage" click on checkbox then click on "Edit data". ? Click on Filter and write Template ID into field "Template Id" and write "body" into field "Message type". After that 31 records will be shown(one record per one locale). ? Click on record for some locale ? Find original template ".html" file that you have taken as backup of current template and locale ? Then copy HTML text of original template into field "Message". ? Click "Save" &gt;&gt; Awaiting for customer to respond 30/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 04/07/2025 &gt;&gt; Explained the customer on how to update the logo image of the specific template &gt;&gt; Customer will test and get back to us next week &gt;&gt; Awaiting for customer to respond 07/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 10/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 14/07/2025 &gt;&gt; As agreed over the call with customer last friday we already emailed to customer that if no response on Monday, we will close the case Monday EOD ---------------------------------------------------------------------------------------------------- Action Plan: Need to find doc - need to create a copy of template - company specific &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:Data:Provided guidance on credential encryption/decryption capabilities.:Educate</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Branding:Different logos possible via separate branding settings.:Educate</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2009806</v>
+        <v>1995733</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>NEOM: Disable the DWP OOTB notification 'Waiting approval' for approver</t>
+          <t>ITSR closed but still showing active in DWP</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Please, we need to disable the DWP OOTB notification on "Waiting approval" for all logged-on users by applying the query on the DB level as mentioned in the below article (see the attached file). https://community.bmc.com/s/article/DWP-How-to-bulk-enable-all-the-DWP-notifications-for-all-user-profiles " Please note that you can refer to case number 01691003.</t>
+          <t>Process #197292 is closed but for user its still showing active in his DWP page. email attached with details.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Problem: 3WE What: Where: When: Extent: ---------------------------------------------------------------------------------------------------- Action Taken: ---------------------------------------------------------------------------------------------------- Action Plan: ---------------------------------------------------------------------------------------------------- Action Owner:</t>
+          <t>Problem: Request in Active Event 3WE What: Closed Request in Active Event Where: DWP - Request When: Request is closed Extent: 1 Request ---------------------------------------------------------------------------------------------------- Action Taken: The Request status was active. Closed the request 11/07/2025 &gt;&gt; Customer re-opened the case and asked there are few other requests that are active, below update shared with the customer: &gt;&gt; I?ve reviewed the DWPC requests, please find below the details to perform manual polling using Postman: &gt;&gt; Method: POST &gt;&gt; Endpoint: {{hostport}}/api/myit-sb/requests/{{requestId}}/poll?async=true &gt;&gt; Example: POST https://qgitsm-dwpcatalog.onbmc.com/api/myit-sb/requests/191376/poll?async=true &gt;&gt; You will also need to authenticate first: &gt;&gt; Method: POST &gt;&gt; Endpoint: https://qgitsm-dwpcatalog.onbmc.com/api/myit-sb/users/login Body: {"id": "your admin user", "password": "your password"} &gt;&gt; DWPC Request IDs that you have shared with us, you will need to add them in the end point URL: Req. 191376 -- Active Req. 199506 -- Active Req. 194478 -- Active REQ000001051580 (DWPC RequestID: 102821) -- Active/Pending Req. 193204 -- Active Req. 197015 -- Active Req. 193250 -- Active REQ000001292552 (DWPC RequestID: 240273) -- Active &gt;&gt; To close the requests, you?ll need to include the corresponding DWPC Request ID in the endpoint URL and run the appropriate call using Postman. &gt;&gt; You can also do the same from the front end via the IS Service Request Table. &gt;&gt; Awaiting for customer to respond 14/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 17/07/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond 18/07/2025 &gt;&gt; Multiple follow ups done and no customer response, hence closing this case 21/07/2025 &gt;&gt; Got closure on the case ---------------------------------------------------------------------------------------------------- Action Plan: Customer to validate &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Notification Template:Disabled 'Waiting approval' notification via DB query.:Customization</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Workflow:Investigate workflow status sync issue in DWP.:R&amp;D</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2009947</v>
+        <v>1996049</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Increase Autoclose DWP Request</t>
+          <t>Request to make DWP url public, first for non-production and then to production</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hello team, in this case, 01972804 , we requested to BMC to increase this value, (OOTB is 2 months). The BMC team, advised us that an upgrade will change this value. Can you increase to 1 year again?</t>
+          <t>Currently most of our techservicehub urls are private (inside VPN) but we have Helix Dashboards public. We requested that change last year under case 01773755 (please if you can refer for the details) We would like to do the similar activity for the DWP (end user), following ones but not the admin. Please let us know if that is possible. DWP URL: https://techservicehub-dev-dwp.onbmc.com/app https://techservicehub-qa-dwp.onbmc.com/app https://techservicehub-dwp.onbmc.com/app</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Problem: Increase Autoclose DWP Request 3WE What: Increase Autoclose DWP Request Where: DWP version 23.3.04 When: Query Extent: Query ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; Refer to the bookmarked mail for solution &gt;&gt; Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case -------------------------------- -------------------------------------------------------------------- Action Owner: TSA for closure</t>
+          <t>Problem: Request to make DWP url public, first for non-production and then to production 3WE What: Request to make DWP url public, first for non-production and then to production Where: dev,QA and Prod When: Extent: Whitelist DWP URL ---------------------------------------------------------------------------------------------------- Action Taken: 13th June: Raised WO0000001484850 for Network Team 16th June: Sent an email to the customer that we are still waiting for an update from Network Team 20/06/2025 &gt;&gt; Followed up on the WO with Network Team and also on the case with the customer &gt;&gt; Awaiting for Network Team to respond 23/06/2025 &gt;&gt; Followed up on the email with the Network Team (*** IMP *** (TalkTalk Communications Ltd "techservicehub-prod") WO0000001484850 | Request to make DWP url public | 01996049) &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for Network Support Team to respond 24/06/2025 &gt;&gt; Network Support Team requested for the teams call with the customer &gt;&gt; Requested the availability for call from the customer &gt;&gt; Awaiting for customer to respond &gt;&gt; Requested Network team to confirm if we can set the call tomorrow at 1:30 PM IST &gt;&gt; Awaiting for NW team to respond. &gt;&gt; RE: *** IMP *** (TalkTalk Communications Ltd "techservicehub-prod") WO0000001484850 | Request to make DWP url public | 01996049 25/06/2025 &gt;&gt; Got closure on the case over the call. Call summary below ? The restrictions for this https://techservicehub-dev-dwp.onbmc.com URL is removed by our Network Team. ? Customer is getting Access Restricted: This environment is restricted. Your source address (IP) is not allowed. Contact your network administrator for further details. For each user different IP is being shown. ? Saleem Savanur checking the issue from Network Side again. ? Post changes were done, on Dev the issue is resolved now. Customer is able to login to Dev Instance all the users. ? But, customer was using: https://techservicehub-dev-dwp.onbmc.com/dwp/user_domain=talktalk due to which they were getting error. ? We gave correct URL: https://techservicehub-dev-dwp.onbmc.com/dwp/?user_domain=talktalk it started working for the customer. ? For all the users the URL is now the Dev One. ? Now, Network Engineer started to remove restriction for the QA, as requested by the customer. ? Okay now QA is also working fine. ? Customer used this one for QA: https://techservicehub-qa-dwp.onbmc.com/dwp/?user_domain=talktalk it worked fine ? Only Dev and QA is done, for Prod they will raise a separate case. ? This case can be closed. &gt;&gt; Got clousre, Closing the case ---------------------------------------------------------------------------------------------------- Action Plan: Waiting for Network Support &gt;&gt; Awaiting for Network Team to respond &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Configuration:Increased autoclose duration to 1 year.:Customization</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Configuration:Guide on making DWP URL public.:Educate</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2010404</v>
+        <v>1996490</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sync the Service Request Status to Closed</t>
+          <t>DWP Catalog Query</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1, Please update the status of the listed Service Requests (SRs) 3337823, 3382522, 3391128 to "Closed." 2, Investigate why these SRs remain in "Active" status despite all related Work Orders (WOs) and fulfillments being marked as completed/Closed in Smart IT. Please reach me out at 7569537548.</t>
+          <t>Dear Support, There is a requirement for downloading an excel file in one of the Services in DWP Catalog for which the fulfillment request is BWF LOB Case Management. What we need is something similar to the Documents Form Element Type. Please see the attached screenshot. This type of field currently supports only PDF. Is there any way to include excel files also in this field? If not, what is the best alternative for accomplishing this requirement. Kindly help. Thanks and regards Ani Sankar</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Problem: Sync the Service Request Status to Closed 3WE What: Please update the status of the listed Service Requests (SRs) 3337823, 3382522, 3391128 to "Closed." Where: Prod When: Happened in past Extent: 3 requests affected ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; Closed from backend &gt;&gt; 3 follow ups done ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
+          <t>Problem: DWP Catalog Query 3WE What: DWP Catalog Query Where: qafco-dev When: when attaching excel in the questionnaire Extent: general query from the customer ---------------------------------------------------------------------------------------------------- Action Taken: 13th June: discussed this with the R&amp;D team and they have confirmed it is not possible. R&amp;D has hardcoded restriction on PDF only. You can refer to the following doc: https://docs.bmc.com/docs/display/dwpMaster2/.Adding+questions+to+a+questionnaire+v23.3.02 Please feel free to raise an idea on https://community.bmc.com/s/all-ideas 1) Alternatively, you can try storing the file somewhere and share a link to it in the questions. 2)You can also try using repeatable questions for your use case. Please refer to the following documentation: https://docs.bmc.com/docs/dwp233/creating-a-repeatable-group-of-questions-1240715470.html You can also try storing the file somewhere and share a link to it in the questions. Please be advised that you are referring to an ootb customization, above approach needs to be tested and validated from your end 16th June: Best is to store the file as a KB article and provide the link so that users can download it from there. There is no other workaround as pdf is the only supported file type for Documents Form Element Types. Please let me know if there is anything else I can help you with or okay to close this case ? 17th June: Follow-up email sent 18th June: Follow-up email sent 19th June: Called and spoke to the customer, they will get back to us tomorrow 23/06/2025 &gt;&gt; Followed up with the customer &gt;&gt; Awaiting for customer to respond &gt;&gt; Got closure on the case &gt;&gt; Closing this case ---------------------------------------------------------------------------------------------------- Action Plan: Waiting for customer's response &gt;&gt; Awaiting for customer to respond ---------------------------------------------------------------------------------------------------- Action Owner: bmc</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>#PBM:SRM:Workflow:Investigate SR status sync issue with Smart IT.:R&amp;D</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>2010514</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Please setup enhanced catalog for sub tenant Tiger Brand Limited on Prod</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Please setup enhanced catalog for sub tenant Tiger Brand Limited on Prod, this has already been done in the lower environments.</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Problem: DWP Catalog section Error 3WE What: Alert pops up when we go from DWPA -&gt; Service Requests -&gt; Catalog sections. Where: Prod - DWP version 25.1.02 | build number: 4 When: Post enhanced catalog configuration Extent: DWP Admin console Steps to replicate: 1. Login to DWP Admin -&gt; Service Requests -&gt; Catalog sectons 2. One alert message will pop up saying "Server Encountered Error" ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; R&amp;D discussion with logs and analysis: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1752221912807?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1752221912807&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1752221912807 &gt;&gt; Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>#PBM:DWP:Multitenancy:Enhanced catalog setup for sub tenant on Prod.:Customization</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>2010532</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Log for DWPC deactivating Service Action needed</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Hi team, today in the morning we saw that the Service Action "Install Software" in DWPC was deactivated for some reason unknown. Noone in our team has a clue why this was changed and who did it. Is there any background log which might be able to have catched this information? Obviously, we re-activated the Service Action as soon as we saw it deactivated, so this is to consider. Please investigate, thx in advance</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Problem: Log for DWPC deactivating Service Action needed 3WE What: Log for DWPC deactivating Service Action needed Where: DWP version 23.3.04 When: Issue happened in past Extent: Issue happened in past ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1752153870505?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1752153870505&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1752153870505 &gt;&gt; Maybe, this service action is mapped to service that was unpublished? &gt;&gt; 3 follow ups ---------------------------------------------------------------------------------------------------- Action Plan: Closong the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>#PBM:DWPC:Log:Investigate logs for deactivation cause.:NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>2010622</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Change the Status to Completed</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Dear Team, Requesting your support to mark the Request ID status to completed. Request ID - 710688 Attached screenshot for your ref</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Problem: Change the Status to Completed 3WE What: Change the Status to Completed Where: Prod - DWP version 23.3.02 When: Issue repported on 10/07 Extent: 1 SR ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; Closed from backend &gt;&gt; Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>#PBM:DWP:Request:Manually updated request status to completed.:NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>2010722</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Users display a deleted broadcast</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Hello support team, Today we created a diffusion by customer request, after a few hours the customer requested to remove it. Therefore we removed it, however it still appears in the DWP portal. We request to remove it, as it is possible that it is not synchronized at some point. Greetings, Iván Hernández</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Problem: 3WE What: Where: When: Extent: ---------------------------------------------------------------------------------------------------- Action Taken: ---------------------------------------------------------------------------------------------------- Action Plan: ---------------------------------------------------------------------------------------------------- Action Owner:</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>#PBM:DWP:Broadcast:Broadcast not removed due to sync issue; check synchronization.:NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>2011223</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>About the error received by users trying to access DWP</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Hello, we are using reCAPTCHA v3. We are encountering the attached error when trying to log in to the Digital Workplace. Sometimes users receive the error twice before successfully logging in, sometimes they log in on the first attempt, and occasionally it takes four errors before they can log in. Do you have any suggestions for resolving this issue?</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Problem: 3WE What: Where: When: Extent: ---------------------------------------------------------------------------------------------------- Action Taken: ---------------------------------------------------------------------------------------------------- Action Plan: ---------------------------------------------------------------------------------------------------- Action Owner:</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>#PBM:DWP:Configuration:Check reCAPTCHA configuration and adjust settings.:Educate</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>2011290</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Comments on DWP showing username</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>We have a question regarding the comments for interactions on DWP. As shown in the screenshot, users create certain comments on DWP interactions. We want to know whether it´s possible that, instead of showing the user´s username that created it, maybe we could show the Default Support Group name to which they are assigned, or some other general field, instead of the name (we want to keep it private). Is this possible? If so, how can we change it? Thank you.</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Problem: Comments on DWP showing username 3WE What: Comments on DWP showing username Where: nexus-sand When: General query Extent: General query ---------------------------------------------------------------------------------------------------- Action Taken: R&amp;D: https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1752235373300?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1752235373300&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1752235373300 &gt;&gt; Not possible &gt;&gt; Customer provided closure ---------------------------------------------------------------------------------------------------- Action Plan: Closing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>#PBM:DWP:Customization:Usernames in comments can be customized via settings.:FAQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>2011555</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>For helixdemoash2481-demo-is.onbmc.com: When I go to enable services in chatbot in the dwpc the page errors out no matter what helix user or browser</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>For helixdemoash2481-demo-is.onbmc.com: When I go to enable services in chatbot in the dwpc the page errors out no matter what helix user or browser</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Problem: Enable in Chatbot in DWPC not loading 3WE What: Enable in Chatbot in DWPC not loading Where: DWP version 25.2.02 When: Issue reported on 11/07 Extent: DWPC services in chatbot ---------------------------------------------------------------------------------------------------- Action Taken: &gt;&gt; https://teams.microsoft.com/l/message/19:155e65c3543c4f79bfc3089446a57a88@thread.tacv2/1752676147954?tenantId=92b796c5-5839-40a6-8dd9-c1fad320c69b&amp;groupId=9f8be3aa-9422-4aaf-a8d3-93bc59b4d469&amp;parentMessageId=1752676147954&amp;teamName=DWP-Backline%20Support&amp;channelName=General&amp;createdTime=1752676147954 &gt;&gt; Added url in IS &gt;&gt; Provided closure ---------------------------------------------------------------------------------------------------- Action Plan: CLosing the case ---------------------------------------------------------------------------------------------------- Action Owner: TSA for closure</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>#PBM:DWPC:Configuration:Page error when enabling services in chatbot; check configuration settings.:NA</t>
+          <t>Gunjan Bondre</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>#PBM:DWP:Fulfillment Request:Excel file support not available; consider alternative field types.:Customization</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added gemini model with model print statement
</commit_message>
<xml_diff>
--- a/pbm_output.xlsx
+++ b/pbm_output.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Request:Change request not visible due to request visibility settings.:R&amp;D</t>
+          <t>#PBM:DWP:Defect:SmartIT/MidTier integration issue;  DWP not displaying customer requests.  Requires investigation.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Approval:Error due to deleted approver profile; needs handling for delegate approvals.:R&amp;D</t>
+          <t>#PBM:DWP:Defect:Internal server error when opening delegate approvals for approvers with deleted profiles;  handling of deleted approver profiles in approval workflow needs to be improved.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:Entitlement:Check entitlement configuration for visibility issues.:Configuration</t>
+          <t>#PBM:DWPA:Entitlement:Entitlement not properly assigned to users; corrected entitlement configuration.:NA</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>#PBM:DWPC:Data:Data tables not visible in form mapping; investigate configuration.:NA</t>
+          <t>#PBM:DWPC:Defect:Dev DWPC forms: Missing data tables in action mapping fixed.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Approval:Investigate why approval status not updated in Catalog.:R&amp;D</t>
+          <t>#PBM:DWP:Workflow:Status update failure in Catalog; workflow investigated and corrected.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Upgrade:Upgrade patch applied to QA without sample data.:NA</t>
+          <t>#PBM:DWP:Upgrade:23.3.04 patch deployed to QA environment excluding sample data, DWPC catalogs, and DWP Studio pages.:NA</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Integration:Investigate DWP-ITSM comment sync issue.:R&amp;D</t>
+          <t>#PBM:DWP:Integration:Investigating DWP-ITSM integration issue; worklog comments not syncing.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Notification Template:Check template activation and cache refresh.:Customization</t>
+          <t>#PBM:DWP:Notification Template:Investigated email template issue; found a rendering problem.  Template corrected.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Workflow:Double quotes in names cause workflow errors; needs masking solution.:R&amp;D</t>
+          <t>#PBM:DWP:Defect:DWP error caused by double quotes in request field; evaluate framework fix to handle special characters.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Branding:Different logos possible via separate branding settings.:Educate</t>
+          <t>#PBM:DWP:Branding:Confirmed separate logos for email template and DWP portal are possible.  Advised on customization steps.:Customization</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Workflow:Investigate workflow status sync issue in DWP.:R&amp;D</t>
+          <t>#PBM:DWP:Defect:UI refresh issue; corrected data display.:R&amp;D</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Configuration:Guide on making DWP URL public.:Educate</t>
+          <t>#PBM:DWP:Request:Request to make DWP URLs public; feasibility assessment needed.:NA</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>#PBM:DWP:Fulfillment Request:Excel file support not available; consider alternative field types.:Customization</t>
+          <t>#PBM:DWP:Customization:Explore adding Excel support to Documents Form Element or suggest alternative solutions.:R&amp;D</t>
         </is>
       </c>
     </row>

</xml_diff>